<commit_message>
sierra leone master data
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/app_detail.xlsx
+++ b/mosip_master/xlsx/app_detail.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Country Details\Madagascar\MDG_Master_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chith\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76BCAAE-CAC0-4208-96CA-C37E4B385F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B367C4-E3AF-44A7-862A-B7B38FE8C1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{281C2C0F-B15E-4327-9F70-1C6D3AF8BEF6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -42,43 +42,43 @@
     <t>is_active</t>
   </si>
   <si>
-    <t>fra</t>
-  </si>
-  <si>
-    <t>Pré-inscription</t>
-  </si>
-  <si>
-    <t>Portail web pour les pré-inscriptions</t>
-  </si>
-  <si>
-    <t>Client d'enregistrement</t>
-  </si>
-  <si>
-    <t>Application de bureau pour les inscriptions</t>
-  </si>
-  <si>
-    <t>Processeur d'enregistrement</t>
-  </si>
-  <si>
-    <t>Demande de processus post-inscription</t>
-  </si>
-  <si>
-    <t>Authentification de l'identité</t>
-  </si>
-  <si>
-    <t>Demande d'authentification de fournisseur de services tiers</t>
-  </si>
-  <si>
-    <t>Contrôle d'identité</t>
-  </si>
-  <si>
-    <t>Portail Web pour la configuration des applications</t>
-  </si>
-  <si>
-    <t>Portail résident</t>
-  </si>
-  <si>
-    <t>Portail Web pour les services de génération de Post ID</t>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>Pre-Registration</t>
+  </si>
+  <si>
+    <t>Web portal for pre-registrations</t>
+  </si>
+  <si>
+    <t>Registration Client</t>
+  </si>
+  <si>
+    <t>Desktop application for Registrations</t>
+  </si>
+  <si>
+    <t>Registration Processor</t>
+  </si>
+  <si>
+    <t>Application for post-registration process</t>
+  </si>
+  <si>
+    <t>ID Authentication</t>
+  </si>
+  <si>
+    <t>Application for third party service provider authentication</t>
+  </si>
+  <si>
+    <t>ID Control</t>
+  </si>
+  <si>
+    <t>Web portal for configuring applications</t>
+  </si>
+  <si>
+    <t>Resident Portal</t>
+  </si>
+  <si>
+    <t>Web portal for Post ID generation services</t>
   </si>
 </sst>
 </file>
@@ -88,21 +88,21 @@
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
       <name val="Cambria"/>
-      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <i/>
-      <sz val="8"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -127,6 +127,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -161,31 +176,16 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FF9A9A9A"/>
       </left>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FF9A9A9A"/>
       </right>
       <top style="medium">
         <color rgb="FFCCCCCC"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FF9A9A9A"/>
       </bottom>
       <diagonal/>
     </border>
@@ -208,25 +208,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -543,31 +547,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49862D56-15E2-46FF-AE03-1427303013ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="27.26953125" customWidth="1"/>
-    <col min="4" max="4" width="41.7265625" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" style="1"/>
+    <col min="5" max="5" width="8.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -576,113 +580,114 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="66" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>10001</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="b">
+      <c r="E2" s="7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" ht="66" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="9">
         <v>10003</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="9" t="b">
+      <c r="E3" s="11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" ht="79" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="9">
         <v>10005</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="9" t="b">
+      <c r="E4" s="11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:5" ht="105" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="9">
         <v>10007</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="9" t="b">
+      <c r="E5" s="11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:5" ht="79" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="9">
         <v>10009</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="9" t="b">
+      <c r="E6" s="11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="54" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:5" ht="66" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="9">
         <v>10011</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="9" t="b">
+      <c r="E7" s="11" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>